<commit_message>
feat: Levels are displayed hierarchically
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/api-spec-template-simple.xlsx
+++ b/src/main/resources/templates/api-spec-template-simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A-01. Code\00. Pino\Java\open-api-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00814D51-9C58-47F0-987B-73A9475C53D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30929E9C-B914-41BC-BE37-5DE05639FED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3B4C957-58BD-4660-9D4A-009DF30C1D6F}"/>
   </bookViews>
@@ -359,10 +359,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>${requestParameter.level}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>${requestParameter.name}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -391,11 +387,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>${responseParameter.level}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>參數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${requestParameter.levelValue}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${responseParameter.levelValue}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -520,7 +520,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -545,23 +545,29 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,7 +886,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -893,66 +899,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2"/>
@@ -962,13 +968,13 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="A8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
@@ -1012,13 +1018,13 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
@@ -1038,20 +1044,20 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1062,22 +1068,22 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="101.25" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1">
       <c r="A18" s="6"/>
@@ -1087,13 +1093,13 @@
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
@@ -1105,25 +1111,25 @@
       <c r="C20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>33</v>
+      <c r="A21" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="D21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2"/>
@@ -1133,22 +1139,22 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" ht="99.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2"/>
@@ -1159,11 +1165,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="A23:E23"/>
@@ -1174,6 +1175,11 @@
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add sequence field
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/api-spec-template-simple.xlsx
+++ b/src/main/resources/templates/api-spec-template-simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A-01. Code\00. Pino\Java\open-api-tool\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30929E9C-B914-41BC-BE37-5DE05639FED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B15A02-F25C-4D37-A043-ADAAD2506592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3B4C957-58BD-4660-9D4A-009DF30C1D6F}"/>
   </bookViews>
@@ -307,10 +307,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LVL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>參數位置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -391,11 +387,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>${requestParameter.levelValue}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>${responseParameter.levelValue}</t>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${requestParameter.sequence}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${responseParameter.sequence}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,29 +545,29 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -886,7 +886,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -899,66 +899,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="B5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2"/>
@@ -968,17 +968,17 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>5</v>
@@ -995,19 +995,19 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1018,17 +1018,17 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>5</v>
@@ -1044,20 +1044,20 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1068,17 +1068,17 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" ht="101.25" customHeight="1">
       <c r="A17" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1093,17 +1093,17 @@
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>5</v>
@@ -1111,25 +1111,25 @@
       <c r="C20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="10"/>
+      <c r="D21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2"/>
@@ -1139,17 +1139,17 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="1:5" ht="99.75" customHeight="1">
       <c r="A24" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -1165,6 +1165,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="A23:E23"/>
@@ -1175,11 +1180,6 @@
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>